<commit_message>
Working on 0_constants case for testing sliced variables on special identity. Problem found (see issue #49)
</commit_message>
<xml_diff>
--- a/default/0_constants/input_data/input_data.xlsx
+++ b/default/0_constants/input_data/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\tests_integration\constants_generation\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\0_constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A0B4C7-D5A7-48E0-A2DC-0323A8D98A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D70C3-1AB9-4B50-AE67-4D3BAFB2196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23390" yWindow="1810" windowWidth="21200" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34820" yWindow="3610" windowWidth="15360" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q" sheetId="1" r:id="rId1"/>
@@ -415,10 +415,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>